<commit_message>
update proforma in/out sheet title to "Results Summary and Inputs"
</commit_message>
<xml_diff>
--- a/proforma/REoptCashFlowTemplateOneParty.xlsx
+++ b/proforma/REoptCashFlowTemplateOneParty.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nlaws/projects/reopt/webtool/reopt_api/proforma/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{29D62633-BA61-794B-850F-759D3B599E4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC6BE6BE-3BCB-3749-A725-284917F56F52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6420" yWindow="660" windowWidth="19480" windowHeight="15540" xr2:uid="{223A6E40-735D-7444-92EC-172CE7C1027A}"/>
   </bookViews>
@@ -37,9 +37,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>Inputs</t>
-  </si>
-  <si>
     <t>Optimal Cash Flow</t>
   </si>
   <si>
@@ -62,6 +59,9 @@
       </rPr>
       <t>Cash Flow</t>
     </r>
+  </si>
+  <si>
+    <t>Results Summary and Inputs</t>
   </si>
 </sst>
 </file>
@@ -513,9 +513,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87637F56-F0CF-934C-8621-C8E7D8CAB5CB}">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
@@ -527,7 +525,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="22" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="6"/>
@@ -554,7 +552,7 @@
   <sheetData>
     <row r="1" spans="1:1" ht="21" customHeight="1">
       <c r="A1" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -578,7 +576,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="21" customHeight="1">
       <c r="A1" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" s="5"/>
     </row>

</xml_diff>

<commit_message>
cleaning up bugs from differences in os vs private
</commit_message>
<xml_diff>
--- a/proforma/REoptCashFlowTemplateOneParty.xlsx
+++ b/proforma/REoptCashFlowTemplateOneParty.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nlaws/projects/reopt/webtool/reopt_api/proforma/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tkwasnik/github/REopt_Lite_API/proforma/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC6BE6BE-3BCB-3749-A725-284917F56F52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04DD33B6-FE04-C749-A601-11F92118D67C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6420" yWindow="660" windowWidth="19480" windowHeight="15540" xr2:uid="{223A6E40-735D-7444-92EC-172CE7C1027A}"/>
   </bookViews>
@@ -517,7 +517,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="43.83203125" customWidth="1"/>
+    <col min="1" max="1" width="74.6640625" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" customWidth="1"/>
     <col min="3" max="3" width="13.83203125" customWidth="1"/>
     <col min="4" max="5" width="24.5" customWidth="1"/>
     <col min="6" max="6" width="27.5" customWidth="1"/>

</xml_diff>